<commit_message>
Mandatory Field validation run sucessful
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/TestData/testData.xlsx
+++ b/src/main/java/com/qa/TestData/testData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8303BD0D-E2A0-4083-ADA3-335480B9E15A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BCD84678-1EE6-4C5C-8AA7-87C864F7CAB8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -820,14 +820,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" customWidth="1"/>
+    <col min="3" max="3" width="55.7109375" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
     <col min="5" max="5" width="21.7109375" customWidth="1"/>
     <col min="6" max="6" width="27.85546875" customWidth="1"/>

</xml_diff>

<commit_message>
Toast message validation complete
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/TestData/testData.xlsx
+++ b/src/main/java/com/qa/TestData/testData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BCD84678-1EE6-4C5C-8AA7-87C864F7CAB8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CBBF8B7B-486F-4A91-8980-E4B8678626C5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -821,17 +821,17 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.7109375" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" customWidth="1"/>
     <col min="6" max="6" width="27.85546875" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" customWidth="1"/>
+    <col min="7" max="7" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -897,7 +897,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Changes done for MandatoryFieldValidation
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/TestData/testData.xlsx
+++ b/src/main/java/com/qa/TestData/testData.xlsx
@@ -3,12 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8303BD0D-E2A0-4083-ADA3-335480B9E15A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9952DF51-8B7A-4F16-B981-42602196ADA5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateSTP" sheetId="1" r:id="rId1"/>
+    <sheet name="PostDetails" sheetId="2" r:id="rId2"/>
+    <sheet name="CreateSTP_Mandatory" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="95">
   <si>
     <t>Full Name</t>
   </si>
@@ -218,6 +220,93 @@
   </si>
   <si>
     <t>On Par</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>YourPost</t>
+  </si>
+  <si>
+    <t>Plant1</t>
+  </si>
+  <si>
+    <t>Plant2</t>
+  </si>
+  <si>
+    <t>Plant3</t>
+  </si>
+  <si>
+    <t>Plant4</t>
+  </si>
+  <si>
+    <t>Plant5</t>
+  </si>
+  <si>
+    <t>Details entered successfully for plant1</t>
+  </si>
+  <si>
+    <t>Details entered successfully for plant2</t>
+  </si>
+  <si>
+    <t>Details entered successfully for plant3</t>
+  </si>
+  <si>
+    <t>Details entered successfully for plant4</t>
+  </si>
+  <si>
+    <t>Details entered successfully for plant5</t>
+  </si>
+  <si>
+    <t>STPName</t>
+  </si>
+  <si>
+    <t>STPShortName</t>
+  </si>
+  <si>
+    <t>STPDescription</t>
+  </si>
+  <si>
+    <t>CommunityOrganizer</t>
+  </si>
+  <si>
+    <t>Nimda1</t>
+  </si>
+  <si>
+    <t>Nimda123</t>
+  </si>
+  <si>
+    <t>Nimda2</t>
+  </si>
+  <si>
+    <t>Nimda223</t>
+  </si>
+  <si>
+    <t>Nimda3</t>
+  </si>
+  <si>
+    <t>Nimda323</t>
+  </si>
+  <si>
+    <t>TEst2</t>
+  </si>
+  <si>
+    <t>Nimda4</t>
+  </si>
+  <si>
+    <t>Nimda423</t>
+  </si>
+  <si>
+    <t>TEst3</t>
+  </si>
+  <si>
+    <t>Nimda5</t>
+  </si>
+  <si>
+    <t>Nimda523</t>
+  </si>
+  <si>
+    <t>Test4</t>
   </si>
 </sst>
 </file>
@@ -820,7 +909,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -1209,4 +1298,164 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7712F75A-E967-442F-8AB7-657D0E82153C}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C087CA4-610E-4A04-B4C6-323422E74A89}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="94.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
commit changes for PostTestValidation and Extent Reports
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/TestData/testData.xlsx
+++ b/src/main/java/com/qa/TestData/testData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B47386CE-1939-4DBB-9FC2-69839695448E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D39315A8-82F5-42EF-9EE2-1DA7D3E15584}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateSTP" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="98">
   <si>
     <t>Full Name</t>
   </si>
@@ -307,6 +307,15 @@
   </si>
   <si>
     <t>Test4</t>
+  </si>
+  <si>
+    <t>STPS</t>
+  </si>
+  <si>
+    <t>gggg</t>
+  </si>
+  <si>
+    <t>hello</t>
   </si>
 </sst>
 </file>
@@ -586,7 +595,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -625,6 +634,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -909,7 +921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -1302,31 +1314,44 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7712F75A-E967-442F-8AB7-657D0E82153C}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="35.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>66</v>
       </c>
       <c r="B1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="20"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>68</v>
       </c>
       <c r="B2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -1334,7 +1359,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>70</v>
       </c>
@@ -1342,7 +1367,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>71</v>
       </c>
@@ -1350,7 +1375,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>72</v>
       </c>
@@ -1359,6 +1384,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
List Page Filter categories
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/TestData/testData.xlsx
+++ b/src/main/java/com/qa/TestData/testData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5274ACD7-C945-4408-9389-393C2CFEC7C8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1E95345B-6F70-49D9-A6EB-F82D0DA590EC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,18 +30,12 @@
     <t>Short Name</t>
   </si>
   <si>
-    <t>community organiser</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
     <t>Experts</t>
   </si>
   <si>
-    <t>Business selector</t>
-  </si>
-  <si>
     <t>Location</t>
   </si>
   <si>
@@ -51,33 +45,12 @@
     <t>Assets</t>
   </si>
   <si>
-    <t>Material</t>
-  </si>
-  <si>
     <t>Application</t>
   </si>
   <si>
-    <t>Project</t>
-  </si>
-  <si>
-    <t>Products and serivces</t>
-  </si>
-  <si>
-    <t>Example</t>
-  </si>
-  <si>
-    <t>Related technology</t>
-  </si>
-  <si>
     <t>Database</t>
   </si>
   <si>
-    <t>Trend</t>
-  </si>
-  <si>
-    <t>Keyword</t>
-  </si>
-  <si>
     <t>Publications By Merck</t>
   </si>
   <si>
@@ -87,12 +60,6 @@
     <t>Patents</t>
   </si>
   <si>
-    <t>competitor</t>
-  </si>
-  <si>
-    <t>Expertise level</t>
-  </si>
-  <si>
     <t>Fields</t>
   </si>
   <si>
@@ -228,12 +195,6 @@
     <t>Test4</t>
   </si>
   <si>
-    <t>Technique Used</t>
-  </si>
-  <si>
-    <t>External collaboration</t>
-  </si>
-  <si>
     <t>asset11</t>
   </si>
   <si>
@@ -285,31 +246,70 @@
     <t>TRL 2</t>
   </si>
   <si>
-    <t>LeadContBlank02011</t>
-  </si>
-  <si>
-    <t>Blank Lead Contact02011</t>
-  </si>
-  <si>
-    <t>BlankDescription02011</t>
-  </si>
-  <si>
-    <t>BlankDesc02011</t>
-  </si>
-  <si>
-    <t>fullNameBlank02011</t>
-  </si>
-  <si>
-    <t>FullName202011</t>
-  </si>
-  <si>
-    <t>Short202011</t>
-  </si>
-  <si>
-    <t>FullName102011</t>
-  </si>
-  <si>
-    <t>Short102011</t>
+    <t>Business Sector</t>
+  </si>
+  <si>
+    <t>Community Organizer</t>
+  </si>
+  <si>
+    <t>Expertise Level</t>
+  </si>
+  <si>
+    <t>Technique</t>
+  </si>
+  <si>
+    <t>Ongoing Projects</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>External Examples</t>
+  </si>
+  <si>
+    <t>Related Technology</t>
+  </si>
+  <si>
+    <t>Materials used</t>
+  </si>
+  <si>
+    <t>Associated Trends</t>
+  </si>
+  <si>
+    <t>Keywords</t>
+  </si>
+  <si>
+    <t>External Collaboration</t>
+  </si>
+  <si>
+    <t>Competitor</t>
+  </si>
+  <si>
+    <t>FullName104011</t>
+  </si>
+  <si>
+    <t>FullName204011</t>
+  </si>
+  <si>
+    <t>Short104011</t>
+  </si>
+  <si>
+    <t>Short204011</t>
+  </si>
+  <si>
+    <t>fullNameBlank04011</t>
+  </si>
+  <si>
+    <t>BlankDesc04011</t>
+  </si>
+  <si>
+    <t>BlankDescription04011</t>
+  </si>
+  <si>
+    <t>Blank Lead Contact04011</t>
+  </si>
+  <si>
+    <t>LeadContBlank04011</t>
   </si>
 </sst>
 </file>
@@ -333,7 +333,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -352,6 +352,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="17">
     <border>
@@ -589,7 +601,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -615,12 +627,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -629,6 +635,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -913,7 +931,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,25 +946,25 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>33</v>
+        <v>12</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -955,17 +973,17 @@
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="3" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -974,62 +992,62 @@
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="1" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="2" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>2</v>
+      <c r="A5" s="19" t="s">
+        <v>75</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>4</v>
+      <c r="A6" s="19" t="s">
+        <v>3</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="1"/>
@@ -1037,12 +1055,12 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="5" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>5</v>
+      <c r="A7" s="19" t="s">
+        <v>74</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="1"/>
@@ -1050,12 +1068,12 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="5" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>6</v>
+      <c r="A8" s="19" t="s">
+        <v>4</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="1"/>
@@ -1063,12 +1081,12 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="5" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
-        <v>7</v>
+      <c r="A9" s="18" t="s">
+        <v>5</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="1"/>
@@ -1076,12 +1094,12 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="5" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>8</v>
+      <c r="A10" s="20" t="s">
+        <v>6</v>
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="1"/>
@@ -1089,12 +1107,12 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="5" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>68</v>
+      <c r="A11" s="20" t="s">
+        <v>77</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="1"/>
@@ -1102,12 +1120,12 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="5" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>9</v>
+      <c r="A12" s="20" t="s">
+        <v>82</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="1"/>
@@ -1115,12 +1133,12 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="5" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
-        <v>10</v>
+      <c r="A13" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="1"/>
@@ -1128,12 +1146,12 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="5" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
-        <v>11</v>
+      <c r="A14" s="20" t="s">
+        <v>78</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="1"/>
@@ -1141,12 +1159,12 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="5" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
-        <v>12</v>
+      <c r="A15" s="20" t="s">
+        <v>79</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="1"/>
@@ -1154,12 +1172,12 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="5" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
-        <v>13</v>
+      <c r="A16" s="20" t="s">
+        <v>80</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="1"/>
@@ -1167,12 +1185,12 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="5" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
-        <v>14</v>
+      <c r="A17" s="20" t="s">
+        <v>81</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="1"/>
@@ -1180,12 +1198,12 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="5" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
-        <v>15</v>
+      <c r="A18" s="20" t="s">
+        <v>8</v>
       </c>
       <c r="B18" s="10"/>
       <c r="C18" s="1"/>
@@ -1193,12 +1211,12 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="5" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
-        <v>16</v>
+      <c r="A19" s="20" t="s">
+        <v>83</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="1"/>
@@ -1206,12 +1224,12 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="5" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
-        <v>17</v>
+      <c r="A20" s="20" t="s">
+        <v>84</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="1"/>
@@ -1219,12 +1237,12 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="5" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
-        <v>18</v>
+      <c r="A21" s="20" t="s">
+        <v>9</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="1"/>
@@ -1232,12 +1250,12 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="5" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
-        <v>19</v>
+      <c r="A22" s="20" t="s">
+        <v>10</v>
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="1"/>
@@ -1245,12 +1263,12 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="5" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
-        <v>69</v>
+      <c r="A23" s="20" t="s">
+        <v>85</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="1"/>
@@ -1258,12 +1276,12 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="5" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
-        <v>20</v>
+      <c r="A24" s="20" t="s">
+        <v>11</v>
       </c>
       <c r="B24" s="10"/>
       <c r="C24" s="1"/>
@@ -1271,12 +1289,12 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="5" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
-        <v>21</v>
+      <c r="A25" s="20" t="s">
+        <v>86</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="1"/>
@@ -1284,12 +1302,12 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="5" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="16" t="s">
-        <v>22</v>
+      <c r="A26" s="21" t="s">
+        <v>76</v>
       </c>
       <c r="B26" s="11"/>
       <c r="C26" s="7"/>
@@ -1297,7 +1315,7 @@
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="8" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1317,50 +1335,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1384,80 +1402,80 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="D1" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
List Page category search
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/TestData/testData.xlsx
+++ b/src/main/java/com/qa/TestData/testData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1E95345B-6F70-49D9-A6EB-F82D0DA590EC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{313E5A43-2DF2-4A63-BBA7-1D7F9815384A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -285,18 +285,6 @@
     <t>Competitor</t>
   </si>
   <si>
-    <t>FullName104011</t>
-  </si>
-  <si>
-    <t>FullName204011</t>
-  </si>
-  <si>
-    <t>Short104011</t>
-  </si>
-  <si>
-    <t>Short204011</t>
-  </si>
-  <si>
     <t>fullNameBlank04011</t>
   </si>
   <si>
@@ -310,6 +298,18 @@
   </si>
   <si>
     <t>LeadContBlank04011</t>
+  </si>
+  <si>
+    <t>FullName104012</t>
+  </si>
+  <si>
+    <t>Short104012</t>
+  </si>
+  <si>
+    <t>FullName204012</t>
+  </si>
+  <si>
+    <t>Short204012</t>
   </si>
 </sst>
 </file>
@@ -931,7 +931,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,17 +973,17 @@
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -992,19 +992,19 @@
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>95</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
code complete without extent reports
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/TestData/testData.xlsx
+++ b/src/main/java/com/qa/TestData/testData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{313E5A43-2DF2-4A63-BBA7-1D7F9815384A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7F658B08-5073-4388-8038-D529DA40CB46}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -195,54 +195,6 @@
     <t>Test4</t>
   </si>
   <si>
-    <t>asset11</t>
-  </si>
-  <si>
-    <t>technique11</t>
-  </si>
-  <si>
-    <t>material11</t>
-  </si>
-  <si>
-    <t>application11</t>
-  </si>
-  <si>
-    <t>project11</t>
-  </si>
-  <si>
-    <t>service11</t>
-  </si>
-  <si>
-    <t>example11</t>
-  </si>
-  <si>
-    <t>tech11</t>
-  </si>
-  <si>
-    <t>Database11</t>
-  </si>
-  <si>
-    <t>trend11</t>
-  </si>
-  <si>
-    <t>Keyword11</t>
-  </si>
-  <si>
-    <t>internal publi11</t>
-  </si>
-  <si>
-    <t>external publi11</t>
-  </si>
-  <si>
-    <t>collab11</t>
-  </si>
-  <si>
-    <t>patent11</t>
-  </si>
-  <si>
-    <t>compet11</t>
-  </si>
-  <si>
     <t>TRL 2</t>
   </si>
   <si>
@@ -285,31 +237,79 @@
     <t>Competitor</t>
   </si>
   <si>
-    <t>fullNameBlank04011</t>
-  </si>
-  <si>
-    <t>BlankDesc04011</t>
-  </si>
-  <si>
-    <t>BlankDescription04011</t>
-  </si>
-  <si>
-    <t>Blank Lead Contact04011</t>
-  </si>
-  <si>
-    <t>LeadContBlank04011</t>
-  </si>
-  <si>
-    <t>FullName104012</t>
-  </si>
-  <si>
-    <t>Short104012</t>
-  </si>
-  <si>
-    <t>FullName204012</t>
-  </si>
-  <si>
-    <t>Short204012</t>
+    <t>Blank Lead Contact07011</t>
+  </si>
+  <si>
+    <t>LeadContBlank07011</t>
+  </si>
+  <si>
+    <t>BlankDescription07011</t>
+  </si>
+  <si>
+    <t>BlankDesc07011</t>
+  </si>
+  <si>
+    <t>fullNameBlank07011</t>
+  </si>
+  <si>
+    <t>FullName107011</t>
+  </si>
+  <si>
+    <t>Short107011</t>
+  </si>
+  <si>
+    <t>FullName207011</t>
+  </si>
+  <si>
+    <t>Short207011</t>
+  </si>
+  <si>
+    <t>compet12</t>
+  </si>
+  <si>
+    <t>patent12</t>
+  </si>
+  <si>
+    <t>collab12</t>
+  </si>
+  <si>
+    <t>external publi12</t>
+  </si>
+  <si>
+    <t>internal publi12</t>
+  </si>
+  <si>
+    <t>Keyword12</t>
+  </si>
+  <si>
+    <t>trend12</t>
+  </si>
+  <si>
+    <t>Database12</t>
+  </si>
+  <si>
+    <t>tech12</t>
+  </si>
+  <si>
+    <t>example12</t>
+  </si>
+  <si>
+    <t>service12</t>
+  </si>
+  <si>
+    <t>project12</t>
+  </si>
+  <si>
+    <t>application12</t>
+  </si>
+  <si>
+    <t>material12</t>
+  </si>
+  <si>
+    <t>technique12</t>
+  </si>
+  <si>
+    <t>asset12</t>
   </si>
 </sst>
 </file>
@@ -931,7 +931,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,17 +973,17 @@
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="3" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -992,19 +992,19 @@
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="1" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1028,7 +1028,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="1"/>
@@ -1060,7 +1060,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="1"/>
@@ -1094,7 +1094,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="5" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1107,12 +1107,12 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="5" t="s">
-        <v>57</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="1"/>
@@ -1120,12 +1120,12 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="5" t="s">
-        <v>58</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="1"/>
@@ -1133,7 +1133,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="5" t="s">
-        <v>59</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1146,12 +1146,12 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="5" t="s">
-        <v>60</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="1"/>
@@ -1159,12 +1159,12 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="5" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="1"/>
@@ -1172,12 +1172,12 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="5" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="1"/>
@@ -1185,12 +1185,12 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="5" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="1"/>
@@ -1198,7 +1198,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="5" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1211,12 +1211,12 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="5" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="1"/>
@@ -1224,12 +1224,12 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="5" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="1"/>
@@ -1237,7 +1237,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="5" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1250,7 +1250,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="5" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1263,12 +1263,12 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="5" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="1"/>
@@ -1276,7 +1276,7 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="5" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1289,12 +1289,12 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="5" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="1"/>
@@ -1302,12 +1302,12 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="5" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="21" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="B26" s="11"/>
       <c r="C26" s="7"/>

</xml_diff>

<commit_message>
Intresting code are added
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/TestData/testData.xlsx
+++ b/src/main/java/com/qa/TestData/testData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D39315A8-82F5-42EF-9EE2-1DA7D3E15584}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{861603B0-E65A-433D-AEFA-CE796E2BF74E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateSTP" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="98">
   <si>
     <t>Full Name</t>
   </si>
@@ -228,36 +228,6 @@
     <t>YourPost</t>
   </si>
   <si>
-    <t>Plant1</t>
-  </si>
-  <si>
-    <t>Plant2</t>
-  </si>
-  <si>
-    <t>Plant3</t>
-  </si>
-  <si>
-    <t>Plant4</t>
-  </si>
-  <si>
-    <t>Plant5</t>
-  </si>
-  <si>
-    <t>Details entered successfully for plant1</t>
-  </si>
-  <si>
-    <t>Details entered successfully for plant2</t>
-  </si>
-  <si>
-    <t>Details entered successfully for plant3</t>
-  </si>
-  <si>
-    <t>Details entered successfully for plant4</t>
-  </si>
-  <si>
-    <t>Details entered successfully for plant5</t>
-  </si>
-  <si>
     <t>STPName</t>
   </si>
   <si>
@@ -270,52 +240,82 @@
     <t>CommunityOrganizer</t>
   </si>
   <si>
-    <t>Nimda1</t>
-  </si>
-  <si>
-    <t>Nimda123</t>
-  </si>
-  <si>
-    <t>Nimda2</t>
-  </si>
-  <si>
-    <t>Nimda223</t>
-  </si>
-  <si>
-    <t>Nimda3</t>
-  </si>
-  <si>
-    <t>Nimda323</t>
-  </si>
-  <si>
-    <t>TEst2</t>
-  </si>
-  <si>
-    <t>Nimda4</t>
-  </si>
-  <si>
-    <t>Nimda423</t>
-  </si>
-  <si>
-    <t>TEst3</t>
-  </si>
-  <si>
-    <t>Nimda5</t>
-  </si>
-  <si>
-    <t>Nimda523</t>
-  </si>
-  <si>
-    <t>Test4</t>
-  </si>
-  <si>
-    <t>STPS</t>
-  </si>
-  <si>
-    <t>gggg</t>
-  </si>
-  <si>
-    <t>hello</t>
+    <t>Master1</t>
+  </si>
+  <si>
+    <t>Master2</t>
+  </si>
+  <si>
+    <t>Master3</t>
+  </si>
+  <si>
+    <t>Master4</t>
+  </si>
+  <si>
+    <t>Master5</t>
+  </si>
+  <si>
+    <t>Details entered successfully for Master1</t>
+  </si>
+  <si>
+    <t>Details entered successfully for Master2</t>
+  </si>
+  <si>
+    <t>Details entered successfully for Master3</t>
+  </si>
+  <si>
+    <t>Details entered successfully for Master4</t>
+  </si>
+  <si>
+    <t>Details entered successfully for Master5</t>
+  </si>
+  <si>
+    <t>Kind1</t>
+  </si>
+  <si>
+    <t>Kind2</t>
+  </si>
+  <si>
+    <t>Kind3</t>
+  </si>
+  <si>
+    <t>Kind4</t>
+  </si>
+  <si>
+    <t>Kind5</t>
+  </si>
+  <si>
+    <t>Kind123</t>
+  </si>
+  <si>
+    <t>Kind124</t>
+  </si>
+  <si>
+    <t>Kind125</t>
+  </si>
+  <si>
+    <t>Kind126</t>
+  </si>
+  <si>
+    <t>Kind127</t>
+  </si>
+  <si>
+    <t>Kind6</t>
+  </si>
+  <si>
+    <t>Kind7</t>
+  </si>
+  <si>
+    <t>Kind8</t>
+  </si>
+  <si>
+    <t>Kind128</t>
+  </si>
+  <si>
+    <t>Kind129</t>
+  </si>
+  <si>
+    <t>Kind130</t>
   </si>
 </sst>
 </file>
@@ -595,7 +595,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -634,9 +634,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1314,89 +1311,73 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7712F75A-E967-442F-8AB7-657D0E82153C}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="35.5703125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>66</v>
       </c>
       <c r="B1" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="D1" s="20"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>73</v>
       </c>
-      <c r="C2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>69</v>
-      </c>
       <c r="B3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>70</v>
-      </c>
       <c r="B4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>71</v>
-      </c>
       <c r="B5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>72</v>
-      </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C1:D1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C087CA4-610E-4A04-B4C6-323422E74A89}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1407,16 +1388,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C1" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D1" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1424,7 +1405,7 @@
         <v>82</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
         <v>41</v>
@@ -1435,10 +1416,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C3" t="s">
         <v>41</v>
@@ -1449,13 +1430,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C4" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
         <v>43</v>
@@ -1463,24 +1444,72 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s">
         <v>90</v>
       </c>
       <c r="C5" t="s">
-        <v>91</v>
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>92</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>93</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>94</v>
+      </c>
+      <c r="B9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Help popup updates
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/TestData/testData.xlsx
+++ b/src/main/java/com/qa/TestData/testData.xlsx
@@ -3,16 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{861603B0-E65A-433D-AEFA-CE796E2BF74E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100800_{6E3DF8A5-C11E-4245-A239-6E30325A92E9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13485" windowHeight="2895" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateSTP" sheetId="1" r:id="rId1"/>
     <sheet name="PostDetails" sheetId="2" r:id="rId2"/>
     <sheet name="CreateSTP_Mandatory" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:I7"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="142">
   <si>
     <t>Full Name</t>
   </si>
@@ -240,82 +241,214 @@
     <t>CommunityOrganizer</t>
   </si>
   <si>
-    <t>Master1</t>
-  </si>
-  <si>
-    <t>Master2</t>
-  </si>
-  <si>
-    <t>Master3</t>
-  </si>
-  <si>
-    <t>Master4</t>
-  </si>
-  <si>
-    <t>Master5</t>
-  </si>
-  <si>
-    <t>Details entered successfully for Master1</t>
-  </si>
-  <si>
-    <t>Details entered successfully for Master2</t>
-  </si>
-  <si>
-    <t>Details entered successfully for Master3</t>
-  </si>
-  <si>
-    <t>Details entered successfully for Master4</t>
-  </si>
-  <si>
-    <t>Details entered successfully for Master5</t>
-  </si>
-  <si>
-    <t>Kind1</t>
-  </si>
-  <si>
-    <t>Kind2</t>
-  </si>
-  <si>
-    <t>Kind3</t>
-  </si>
-  <si>
-    <t>Kind4</t>
-  </si>
-  <si>
-    <t>Kind5</t>
-  </si>
-  <si>
-    <t>Kind123</t>
-  </si>
-  <si>
-    <t>Kind124</t>
-  </si>
-  <si>
-    <t>Kind125</t>
-  </si>
-  <si>
-    <t>Kind126</t>
-  </si>
-  <si>
-    <t>Kind127</t>
-  </si>
-  <si>
-    <t>Kind6</t>
-  </si>
-  <si>
-    <t>Kind7</t>
-  </si>
-  <si>
-    <t>Kind8</t>
-  </si>
-  <si>
-    <t>Kind128</t>
-  </si>
-  <si>
-    <t>Kind129</t>
-  </si>
-  <si>
-    <t>Kind130</t>
+    <t>Quality1</t>
+  </si>
+  <si>
+    <t>Quality2</t>
+  </si>
+  <si>
+    <t>Quality3</t>
+  </si>
+  <si>
+    <t>Quality4</t>
+  </si>
+  <si>
+    <t>Quality5</t>
+  </si>
+  <si>
+    <t>Quality6</t>
+  </si>
+  <si>
+    <t>Quality7</t>
+  </si>
+  <si>
+    <t>Quality8</t>
+  </si>
+  <si>
+    <t>Quality9</t>
+  </si>
+  <si>
+    <t>Quality10</t>
+  </si>
+  <si>
+    <t>Quality11</t>
+  </si>
+  <si>
+    <t>Quality12</t>
+  </si>
+  <si>
+    <t>Quality13</t>
+  </si>
+  <si>
+    <t>Quality14</t>
+  </si>
+  <si>
+    <t>Quality15</t>
+  </si>
+  <si>
+    <t>Quality16</t>
+  </si>
+  <si>
+    <t>Quality123</t>
+  </si>
+  <si>
+    <t>Quality124</t>
+  </si>
+  <si>
+    <t>Quality125</t>
+  </si>
+  <si>
+    <t>Quality126</t>
+  </si>
+  <si>
+    <t>Quality127</t>
+  </si>
+  <si>
+    <t>Quality128</t>
+  </si>
+  <si>
+    <t>Quality129</t>
+  </si>
+  <si>
+    <t>Quality130</t>
+  </si>
+  <si>
+    <t>Quality131</t>
+  </si>
+  <si>
+    <t>Quality132</t>
+  </si>
+  <si>
+    <t>Quality133</t>
+  </si>
+  <si>
+    <t>Quality134</t>
+  </si>
+  <si>
+    <t>Quality135</t>
+  </si>
+  <si>
+    <t>Quality136</t>
+  </si>
+  <si>
+    <t>Quality137</t>
+  </si>
+  <si>
+    <t>Quality138</t>
+  </si>
+  <si>
+    <t>TestData1</t>
+  </si>
+  <si>
+    <t>TestData2</t>
+  </si>
+  <si>
+    <t>TestData3</t>
+  </si>
+  <si>
+    <t>TestData4</t>
+  </si>
+  <si>
+    <t>TestData5</t>
+  </si>
+  <si>
+    <t>TestData6</t>
+  </si>
+  <si>
+    <t>TestData7</t>
+  </si>
+  <si>
+    <t>TestData8</t>
+  </si>
+  <si>
+    <t>TestData9</t>
+  </si>
+  <si>
+    <t>TestData10</t>
+  </si>
+  <si>
+    <t>TestData11</t>
+  </si>
+  <si>
+    <t>TestData12</t>
+  </si>
+  <si>
+    <t>TestData13</t>
+  </si>
+  <si>
+    <t>Details entered successfully for TestData1</t>
+  </si>
+  <si>
+    <t>Details entered successfully for TestData2</t>
+  </si>
+  <si>
+    <t>Details entered successfully for TestData3</t>
+  </si>
+  <si>
+    <t>Details entered successfully for TestData4</t>
+  </si>
+  <si>
+    <t>Details entered successfully for TestData5</t>
+  </si>
+  <si>
+    <t>Details entered successfully for TestData6</t>
+  </si>
+  <si>
+    <t>Details entered successfully for TestData7</t>
+  </si>
+  <si>
+    <t>Details entered successfully for TestData8</t>
+  </si>
+  <si>
+    <t>Details entered successfully for TestData9</t>
+  </si>
+  <si>
+    <t>Details entered successfully for TestData10</t>
+  </si>
+  <si>
+    <t>Details entered successfully for TestData11</t>
+  </si>
+  <si>
+    <t>Details entered successfully for TestData12</t>
+  </si>
+  <si>
+    <t>Details entered successfully for TestData13</t>
+  </si>
+  <si>
+    <t>SuccessStoriesData</t>
+  </si>
+  <si>
+    <t>fullname104018</t>
+  </si>
+  <si>
+    <t>fullname104011</t>
+  </si>
+  <si>
+    <t>fullname104012</t>
+  </si>
+  <si>
+    <t>fullname104013</t>
+  </si>
+  <si>
+    <t>fullname104014</t>
+  </si>
+  <si>
+    <t>fullname104015</t>
+  </si>
+  <si>
+    <t>fullname104016</t>
+  </si>
+  <si>
+    <t>fullname104017</t>
+  </si>
+  <si>
+    <t>fullName107011</t>
+  </si>
+  <si>
+    <t>fullName108012</t>
+  </si>
+  <si>
+    <t>fullName108013</t>
   </si>
 </sst>
 </file>
@@ -918,7 +1051,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -1311,60 +1444,164 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7712F75A-E967-442F-8AB7-657D0E82153C}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>66</v>
       </c>
       <c r="B1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="C2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>105</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="C3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="C4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>107</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="C5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>108</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>121</v>
+      </c>
+      <c r="C6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1374,10 +1611,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C087CA4-610E-4A04-B4C6-323422E74A89}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D9"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1402,10 +1639,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C2" t="s">
         <v>41</v>
@@ -1416,10 +1653,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s">
         <v>41</v>
@@ -1430,10 +1667,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C4" t="s">
         <v>41</v>
@@ -1444,10 +1681,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C5" t="s">
         <v>41</v>
@@ -1458,10 +1695,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C6" t="s">
         <v>41</v>
@@ -1472,10 +1709,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="B7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C7" t="s">
         <v>41</v>
@@ -1486,10 +1723,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C8" t="s">
         <v>41</v>
@@ -1500,16 +1737,80 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="B9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C9" t="s">
         <v>41</v>
       </c>
       <c r="D9" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reverted and validated the git conflicts
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/TestData/testData.xlsx
+++ b/src/main/java/com/qa/TestData/testData.xlsx
@@ -3,16 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3B045C15-767A-4A97-9751-E3DADEFEBD7C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100800_{8B760FF7-5FF0-4B2F-89A8-06581052EDD5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10710" windowHeight="5895" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateSTP" sheetId="1" r:id="rId1"/>
     <sheet name="PostDetails" sheetId="2" r:id="rId2"/>
     <sheet name="CreateSTP_Mandatory" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:J17"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="150">
   <si>
     <t>Full Name</t>
   </si>
@@ -114,36 +115,6 @@
     <t>YourPost</t>
   </si>
   <si>
-    <t>Plant1</t>
-  </si>
-  <si>
-    <t>Plant2</t>
-  </si>
-  <si>
-    <t>Plant3</t>
-  </si>
-  <si>
-    <t>Plant4</t>
-  </si>
-  <si>
-    <t>Plant5</t>
-  </si>
-  <si>
-    <t>Details entered successfully for plant1</t>
-  </si>
-  <si>
-    <t>Details entered successfully for plant2</t>
-  </si>
-  <si>
-    <t>Details entered successfully for plant3</t>
-  </si>
-  <si>
-    <t>Details entered successfully for plant4</t>
-  </si>
-  <si>
-    <t>Details entered successfully for plant5</t>
-  </si>
-  <si>
     <t>STPName</t>
   </si>
   <si>
@@ -156,45 +127,6 @@
     <t>CommunityOrganizer</t>
   </si>
   <si>
-    <t>Nimda1</t>
-  </si>
-  <si>
-    <t>Nimda123</t>
-  </si>
-  <si>
-    <t>Nimda2</t>
-  </si>
-  <si>
-    <t>Nimda223</t>
-  </si>
-  <si>
-    <t>Nimda3</t>
-  </si>
-  <si>
-    <t>Nimda323</t>
-  </si>
-  <si>
-    <t>TEst2</t>
-  </si>
-  <si>
-    <t>Nimda4</t>
-  </si>
-  <si>
-    <t>Nimda423</t>
-  </si>
-  <si>
-    <t>TEst3</t>
-  </si>
-  <si>
-    <t>Nimda5</t>
-  </si>
-  <si>
-    <t>Nimda523</t>
-  </si>
-  <si>
-    <t>Test4</t>
-  </si>
-  <si>
     <t>application11</t>
   </si>
   <si>
@@ -313,6 +245,234 @@
   </si>
   <si>
     <t>trend12</t>
+  </si>
+  <si>
+    <t>Swift1</t>
+  </si>
+  <si>
+    <t>Swift2</t>
+  </si>
+  <si>
+    <t>Swift3</t>
+  </si>
+  <si>
+    <t>Swift4</t>
+  </si>
+  <si>
+    <t>Swift5</t>
+  </si>
+  <si>
+    <t>Swift6</t>
+  </si>
+  <si>
+    <t>Swift7</t>
+  </si>
+  <si>
+    <t>Swift8</t>
+  </si>
+  <si>
+    <t>Swift9</t>
+  </si>
+  <si>
+    <t>Swift10</t>
+  </si>
+  <si>
+    <t>Swift11</t>
+  </si>
+  <si>
+    <t>Swift12</t>
+  </si>
+  <si>
+    <t>Swift13</t>
+  </si>
+  <si>
+    <t>Swift14</t>
+  </si>
+  <si>
+    <t>Swift15</t>
+  </si>
+  <si>
+    <t>Swift16</t>
+  </si>
+  <si>
+    <t>Details entered successfully for Swift1</t>
+  </si>
+  <si>
+    <t>Details entered successfully for Swift6</t>
+  </si>
+  <si>
+    <t>Details entered successfully for Swift7</t>
+  </si>
+  <si>
+    <t>Details entered successfully for Swift8</t>
+  </si>
+  <si>
+    <t>Details entered successfully for Swift9</t>
+  </si>
+  <si>
+    <t>Details entered successfully for Swift10</t>
+  </si>
+  <si>
+    <t>Details entered successfully for Swift11</t>
+  </si>
+  <si>
+    <t>Details entered successfully for Swift12</t>
+  </si>
+  <si>
+    <t>Details entered successfully for Swift13</t>
+  </si>
+  <si>
+    <t>Details entered successfully for Swift14</t>
+  </si>
+  <si>
+    <t>Details entered successfully for Swift15</t>
+  </si>
+  <si>
+    <t>Details entered successfully for Swift16</t>
+  </si>
+  <si>
+    <t>Details entered successfully for Swift2</t>
+  </si>
+  <si>
+    <t>Details entered successfully for Swift3</t>
+  </si>
+  <si>
+    <t>Details entered successfully for Swift4</t>
+  </si>
+  <si>
+    <t>Details entered successfully for Swift5</t>
+  </si>
+  <si>
+    <t>Details entered successfully for Swift17</t>
+  </si>
+  <si>
+    <t>Details entered successfully for Swift18</t>
+  </si>
+  <si>
+    <t>Details entered successfully for Swift19</t>
+  </si>
+  <si>
+    <t>Details entered successfully for Swift20</t>
+  </si>
+  <si>
+    <t>Swift17</t>
+  </si>
+  <si>
+    <t>Swift18</t>
+  </si>
+  <si>
+    <t>Swift19</t>
+  </si>
+  <si>
+    <t>Swift20</t>
+  </si>
+  <si>
+    <t>Ferrari1</t>
+  </si>
+  <si>
+    <t>Ferrari2</t>
+  </si>
+  <si>
+    <t>Ferrari3</t>
+  </si>
+  <si>
+    <t>Ferrari4</t>
+  </si>
+  <si>
+    <t>Ferrari5</t>
+  </si>
+  <si>
+    <t>Ferrari6</t>
+  </si>
+  <si>
+    <t>Ferrari7</t>
+  </si>
+  <si>
+    <t>Ferrari8</t>
+  </si>
+  <si>
+    <t>Ferrari9</t>
+  </si>
+  <si>
+    <t>Ferrari10</t>
+  </si>
+  <si>
+    <t>Ferrari11</t>
+  </si>
+  <si>
+    <t>Ferrari12</t>
+  </si>
+  <si>
+    <t>Ferrari13</t>
+  </si>
+  <si>
+    <t>Ferrari14</t>
+  </si>
+  <si>
+    <t>Ferrari15</t>
+  </si>
+  <si>
+    <t>Ferrari16</t>
+  </si>
+  <si>
+    <t>Ferrari17</t>
+  </si>
+  <si>
+    <t>Ferrari18</t>
+  </si>
+  <si>
+    <t>Ferrari123</t>
+  </si>
+  <si>
+    <t>Ferrari124</t>
+  </si>
+  <si>
+    <t>Ferrari125</t>
+  </si>
+  <si>
+    <t>Ferrari126</t>
+  </si>
+  <si>
+    <t>Ferrari127</t>
+  </si>
+  <si>
+    <t>Ferrari128</t>
+  </si>
+  <si>
+    <t>Ferrari129</t>
+  </si>
+  <si>
+    <t>Ferrari130</t>
+  </si>
+  <si>
+    <t>Ferrari131</t>
+  </si>
+  <si>
+    <t>Ferrari132</t>
+  </si>
+  <si>
+    <t>Ferrari133</t>
+  </si>
+  <si>
+    <t>Ferrari134</t>
+  </si>
+  <si>
+    <t>Ferrari135</t>
+  </si>
+  <si>
+    <t>Ferrari136</t>
+  </si>
+  <si>
+    <t>Ferrari137</t>
+  </si>
+  <si>
+    <t>Ferrari138</t>
+  </si>
+  <si>
+    <t>Ferrari139</t>
+  </si>
+  <si>
+    <t>Ferrari140</t>
   </si>
 </sst>
 </file>
@@ -933,7 +1093,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -976,17 +1136,17 @@
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="3" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -995,19 +1155,19 @@
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="1" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1031,7 +1191,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="1"/>
@@ -1042,10 +1202,10 @@
         <v>18</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1058,12 +1218,12 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="5" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="1"/>
@@ -1097,7 +1257,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="5" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1110,12 +1270,12 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="5" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="1"/>
@@ -1123,12 +1283,12 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="5" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="1"/>
@@ -1136,7 +1296,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="5" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1149,12 +1309,12 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="5" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="1"/>
@@ -1162,12 +1322,12 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="5" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="1"/>
@@ -1175,12 +1335,12 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="5" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="1"/>
@@ -1188,12 +1348,12 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="5" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="1"/>
@@ -1201,7 +1361,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="5" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1214,12 +1374,12 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="5" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="1"/>
@@ -1227,12 +1387,12 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="5" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="1"/>
@@ -1240,7 +1400,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="5" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1253,7 +1413,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="5" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1266,12 +1426,12 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="5" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="1"/>
@@ -1279,7 +1439,7 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="5" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1292,12 +1452,12 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="5" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="1"/>
@@ -1305,12 +1465,12 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="5" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="21" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="B26" s="11"/>
       <c r="C26" s="7"/>
@@ -1328,10 +1488,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7712F75A-E967-442F-8AB7-657D0E82153C}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1346,42 +1506,162 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>110</v>
+      </c>
+      <c r="B18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>111</v>
+      </c>
+      <c r="B19" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>112</v>
+      </c>
+      <c r="B20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>113</v>
+      </c>
+      <c r="B21" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1391,10 +1671,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C087CA4-610E-4A04-B4C6-323422E74A89}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D2" sqref="D2:D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1405,24 +1685,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>132</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
@@ -1433,10 +1713,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>115</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>133</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
@@ -1447,13 +1727,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>134</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
         <v>23</v>
@@ -1461,24 +1741,405 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>117</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>135</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>118</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>136</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" t="s">
+        <v>140</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11" t="s">
+        <v>141</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>124</v>
+      </c>
+      <c r="B12" t="s">
+        <v>142</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>125</v>
+      </c>
+      <c r="B13" t="s">
+        <v>143</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>126</v>
+      </c>
+      <c r="B14" t="s">
+        <v>144</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>127</v>
+      </c>
+      <c r="B15" t="s">
+        <v>145</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B16" t="s">
+        <v>146</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>129</v>
+      </c>
+      <c r="B17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>130</v>
+      </c>
+      <c r="B18" t="s">
+        <v>148</v>
+      </c>
+      <c r="C18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>131</v>
+      </c>
+      <c r="B19" t="s">
+        <v>149</v>
+      </c>
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D56" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Help pop-up updates
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/TestData/testData.xlsx
+++ b/src/main/java/com/qa/TestData/testData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3B045C15-767A-4A97-9751-E3DADEFEBD7C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F7BFAC32-BF27-44A1-910D-8DA99EF08329}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,9 +51,6 @@
     <t>Database</t>
   </si>
   <si>
-    <t>Publications By Merck</t>
-  </si>
-  <si>
     <t>Review articles of outside world</t>
   </si>
   <si>
@@ -63,21 +60,6 @@
     <t>Fields</t>
   </si>
   <si>
-    <t>Data1</t>
-  </si>
-  <si>
-    <t>Data2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data3 </t>
-  </si>
-  <si>
-    <t>Data4</t>
-  </si>
-  <si>
-    <t>Data5</t>
-  </si>
-  <si>
     <t>Kushalappa</t>
   </si>
   <si>
@@ -90,9 +72,6 @@
     <t>This is a valid Mandatory Fields scenario. It is supposed give a toast message "STP created successfully!"</t>
   </si>
   <si>
-    <t>Data6</t>
-  </si>
-  <si>
     <t>sharath sethu</t>
   </si>
   <si>
@@ -270,9 +249,6 @@
     <t>Competitor</t>
   </si>
   <si>
-    <t>ukumar1</t>
-  </si>
-  <si>
     <t>asset12</t>
   </si>
   <si>
@@ -297,22 +273,46 @@
     <t>fullNameBlank09011</t>
   </si>
   <si>
-    <t>FullName109011</t>
-  </si>
-  <si>
-    <t>Short109011</t>
-  </si>
-  <si>
-    <t>FullName209011</t>
-  </si>
-  <si>
-    <t>Short209011</t>
-  </si>
-  <si>
     <t>Database12</t>
   </si>
   <si>
     <t>trend12</t>
+  </si>
+  <si>
+    <t>Publications By Merck/EMD</t>
+  </si>
+  <si>
+    <t>FullName110012</t>
+  </si>
+  <si>
+    <t>FullName210012</t>
+  </si>
+  <si>
+    <t>Short110012</t>
+  </si>
+  <si>
+    <t>Short210012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uday </t>
+  </si>
+  <si>
+    <t>Data1(Negative case)</t>
+  </si>
+  <si>
+    <t>Data2(Negative Case)</t>
+  </si>
+  <si>
+    <t>Data3 (Negative Case)</t>
+  </si>
+  <si>
+    <t>Data4 (Negative Case)</t>
+  </si>
+  <si>
+    <t>Data5(Mandatory fields)</t>
+  </si>
+  <si>
+    <t>Data6 (All Fields)</t>
   </si>
 </sst>
 </file>
@@ -934,7 +934,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -949,25 +949,25 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>13</v>
+        <v>91</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>15</v>
+        <v>93</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>16</v>
+        <v>94</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>17</v>
+        <v>95</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>22</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -976,17 +976,17 @@
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -995,19 +995,19 @@
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="1" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1016,36 +1016,36 @@
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1058,12 +1058,12 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="5" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="1"/>
@@ -1071,7 +1071,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="5" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1084,7 +1084,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="5" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1097,7 +1097,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="5" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1110,12 +1110,12 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="5" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="1"/>
@@ -1123,12 +1123,12 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="5" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="1"/>
@@ -1136,7 +1136,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="5" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1149,12 +1149,12 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="1"/>
@@ -1162,12 +1162,12 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="5" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="1"/>
@@ -1175,12 +1175,12 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="5" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="1"/>
@@ -1188,12 +1188,12 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="5" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="1"/>
@@ -1201,7 +1201,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="5" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1214,12 +1214,12 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="5" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="1"/>
@@ -1227,12 +1227,12 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="5" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="1"/>
@@ -1240,12 +1240,12 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="5" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="1"/>
@@ -1253,12 +1253,12 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="5" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="1"/>
@@ -1266,12 +1266,12 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="5" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="1"/>
@@ -1279,12 +1279,12 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="5" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B24" s="10"/>
       <c r="C24" s="1"/>
@@ -1292,12 +1292,12 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="5" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="1"/>
@@ -1305,12 +1305,12 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="5" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="21" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B26" s="11"/>
       <c r="C26" s="7"/>
@@ -1318,7 +1318,7 @@
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="8" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1338,50 +1338,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1405,80 +1405,80 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commiting Extent reports update
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/TestData/testData.xlsx
+++ b/src/main/java/com/qa/TestData/testData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F7BFAC32-BF27-44A1-910D-8DA99EF08329}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8A7B9B88-EC36-4061-AA6F-302472B006A1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="98">
   <si>
     <t>Full Name</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Fields</t>
   </si>
   <si>
-    <t>Kushalappa</t>
-  </si>
-  <si>
     <t>This is a blank Full name case. It is supposed to give a toast message "Required Full Name"</t>
   </si>
   <si>
@@ -282,21 +279,6 @@
     <t>Publications By Merck/EMD</t>
   </si>
   <si>
-    <t>FullName110012</t>
-  </si>
-  <si>
-    <t>FullName210012</t>
-  </si>
-  <si>
-    <t>Short110012</t>
-  </si>
-  <si>
-    <t>Short210012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uday </t>
-  </si>
-  <si>
     <t>Data1(Negative case)</t>
   </si>
   <si>
@@ -313,6 +295,27 @@
   </si>
   <si>
     <t>Data6 (All Fields)</t>
+  </si>
+  <si>
+    <t>FullName214011</t>
+  </si>
+  <si>
+    <t>Short214011</t>
+  </si>
+  <si>
+    <t>ukumar1</t>
+  </si>
+  <si>
+    <t>Uday kumar</t>
+  </si>
+  <si>
+    <t>Uday Kumar</t>
+  </si>
+  <si>
+    <t>FullName114014</t>
+  </si>
+  <si>
+    <t>Short114014</t>
   </si>
 </sst>
 </file>
@@ -368,7 +371,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -600,11 +603,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -651,6 +663,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -931,10 +944,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,108 +960,111 @@
     <col min="7" max="7" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="H5" s="22" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>3</v>
       </c>
@@ -1058,12 +1074,15 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="H6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="1"/>
@@ -1071,10 +1090,10 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>4</v>
       </c>
@@ -1084,10 +1103,10 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>5</v>
       </c>
@@ -1097,10 +1116,10 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>6</v>
       </c>
@@ -1110,12 +1129,12 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="1"/>
@@ -1123,12 +1142,12 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="1"/>
@@ -1136,10 +1155,10 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>7</v>
       </c>
@@ -1149,12 +1168,12 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="1"/>
@@ -1162,12 +1181,12 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="1"/>
@@ -1175,12 +1194,12 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="1"/>
@@ -1188,12 +1207,12 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="1"/>
@@ -1201,7 +1220,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1214,12 +1233,12 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="1"/>
@@ -1227,12 +1246,12 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="1"/>
@@ -1240,12 +1259,12 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="1"/>
@@ -1253,7 +1272,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1266,12 +1285,12 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="1"/>
@@ -1279,7 +1298,7 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1292,12 +1311,12 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="1"/>
@@ -1305,12 +1324,12 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B26" s="11"/>
       <c r="C26" s="7"/>
@@ -1318,7 +1337,7 @@
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1338,50 +1357,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
         <v>21</v>
-      </c>
-      <c r="B1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1405,80 +1424,80 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>35</v>
-      </c>
-      <c r="D1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
         <v>37</v>
       </c>
-      <c r="B2" t="s">
-        <v>38</v>
-      </c>
       <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
         <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
         <v>39</v>
       </c>
-      <c r="B3" t="s">
-        <v>40</v>
-      </c>
       <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
         <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" t="s">
         <v>41</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>42</v>
       </c>
-      <c r="C4" t="s">
-        <v>43</v>
-      </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" t="s">
         <v>44</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>45</v>
-      </c>
-      <c r="C5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
         <v>47</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>48</v>
-      </c>
-      <c r="C6" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Success Stories News and STP News Validation
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/TestData/testData.xlsx
+++ b/src/main/java/com/qa/TestData/testData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100800_{6E3DF8A5-C11E-4245-A239-6E30325A92E9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100800_{3A61E9A0-87C1-46BD-9A1F-E68304430AD0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13485" windowHeight="2895" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14730" windowHeight="1965" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateSTP" sheetId="1" r:id="rId1"/>
@@ -1446,14 +1446,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7712F75A-E967-442F-8AB7-657D0E82153C}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="39.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Extent report for regression.xml suite
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/TestData/testData.xlsx
+++ b/src/main/java/com/qa/TestData/testData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100800_{05DC639B-5770-4DCE-95A0-7F1F46BD6883}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D6CF6727-53B0-407A-A159-424E1A1F737A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10845" windowHeight="2640" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10845" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateSTP" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,6 @@
     <sheet name="CreateSTP_Mandatory" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:C6"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="151">
   <si>
     <t>Full Name</t>
   </si>
@@ -52,9 +51,6 @@
     <t>Database</t>
   </si>
   <si>
-    <t>Publications By Merck</t>
-  </si>
-  <si>
     <t>Review articles of outside world</t>
   </si>
   <si>
@@ -127,9 +123,6 @@
     <t>CommunityOrganizer</t>
   </si>
   <si>
-    <t>application11</t>
-  </si>
-  <si>
     <t>project11</t>
   </si>
   <si>
@@ -229,18 +222,6 @@
     <t>fullNameBlank09011</t>
   </si>
   <si>
-    <t>FullName109011</t>
-  </si>
-  <si>
-    <t>Short109011</t>
-  </si>
-  <si>
-    <t>FullName209011</t>
-  </si>
-  <si>
-    <t>Short209011</t>
-  </si>
-  <si>
     <t>Database12</t>
   </si>
   <si>
@@ -473,6 +454,27 @@
   </si>
   <si>
     <t>Ferrari140</t>
+  </si>
+  <si>
+    <t>Publications by Merck/EMD</t>
+  </si>
+  <si>
+    <t>Uday Kumar</t>
+  </si>
+  <si>
+    <t>Short117011</t>
+  </si>
+  <si>
+    <t>FullName217011</t>
+  </si>
+  <si>
+    <t>Short217011</t>
+  </si>
+  <si>
+    <t>FullName117012</t>
+  </si>
+  <si>
+    <t>application12</t>
   </si>
 </sst>
 </file>
@@ -528,7 +530,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -760,11 +762,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -811,6 +822,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1091,10 +1103,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1107,108 +1119,111 @@
     <col min="7" max="7" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="C1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="E1" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="F1" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="16" t="s">
-        <v>17</v>
-      </c>
       <c r="G1" s="17" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
-        <v>68</v>
+        <v>149</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>69</v>
+        <v>146</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="H5" s="22" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>3</v>
       </c>
@@ -1218,12 +1233,15 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="H6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="1"/>
@@ -1231,10 +1249,10 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>4</v>
       </c>
@@ -1244,10 +1262,10 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>5</v>
       </c>
@@ -1257,10 +1275,10 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>6</v>
       </c>
@@ -1270,12 +1288,12 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="1"/>
@@ -1283,12 +1301,12 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="1"/>
@@ -1296,10 +1314,10 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>7</v>
       </c>
@@ -1309,12 +1327,12 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="1"/>
@@ -1322,12 +1340,12 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="1"/>
@@ -1335,12 +1353,12 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="1"/>
@@ -1348,12 +1366,12 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="1"/>
@@ -1361,7 +1379,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1374,12 +1392,12 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="1"/>
@@ -1387,12 +1405,12 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="5" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="1"/>
@@ -1400,12 +1418,12 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
-        <v>9</v>
+        <v>144</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="1"/>
@@ -1413,12 +1431,12 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="1"/>
@@ -1426,12 +1444,12 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="1"/>
@@ -1439,12 +1457,12 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B24" s="10"/>
       <c r="C24" s="1"/>
@@ -1452,12 +1470,12 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="1"/>
@@ -1465,12 +1483,12 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B26" s="11"/>
       <c r="C26" s="7"/>
@@ -1478,7 +1496,7 @@
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1498,170 +1516,170 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
         <v>28</v>
-      </c>
-      <c r="B1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B6" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B7" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B10" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B12" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B13" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B14" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B15" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B16" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B17" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B18" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B19" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B20" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B21" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1673,7 +1691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C087CA4-610E-4A04-B4C6-323422E74A89}">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D57"/>
     </sheetView>
   </sheetViews>
@@ -1685,461 +1703,461 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
         <v>30</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>31</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>32</v>
-      </c>
-      <c r="D1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B4" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B6" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B7" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B8" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B9" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B10" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B11" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B12" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B13" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B14" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B15" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B16" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B17" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B18" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B19" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="40" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="44" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D46" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="48" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="51" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="53" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D53" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="55" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="56" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="57" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D57" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test.log to Home Page
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/TestData/testData.xlsx
+++ b/src/main/java/com/qa/TestData/testData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D6CF6727-53B0-407A-A159-424E1A1F737A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{17BF5642-E7A1-4A85-97B6-36B048F52CCB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10845" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="150">
   <si>
     <t>Full Name</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Data5</t>
   </si>
   <si>
-    <t>Kushalappa</t>
-  </si>
-  <si>
     <t>This is a blank Full name case. It is supposed to give a toast message "Required Full Name"</t>
   </si>
   <si>
@@ -462,19 +459,19 @@
     <t>Uday Kumar</t>
   </si>
   <si>
-    <t>Short117011</t>
-  </si>
-  <si>
-    <t>FullName217011</t>
-  </si>
-  <si>
-    <t>Short217011</t>
-  </si>
-  <si>
-    <t>FullName117012</t>
-  </si>
-  <si>
     <t>application12</t>
+  </si>
+  <si>
+    <t>FullName117016</t>
+  </si>
+  <si>
+    <t>Short117016</t>
+  </si>
+  <si>
+    <t>FullName217016</t>
+  </si>
+  <si>
+    <t>Short217016</t>
   </si>
 </sst>
 </file>
@@ -1105,8 +1102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1139,7 +1136,7 @@
         <v>16</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1148,17 +1145,17 @@
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1167,19 +1164,19 @@
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -1188,39 +1185,39 @@
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H5" s="22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1233,15 +1230,15 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="1"/>
@@ -1249,7 +1246,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1262,7 +1259,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1275,7 +1272,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1288,12 +1285,12 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="1"/>
@@ -1301,12 +1298,12 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="1"/>
@@ -1314,7 +1311,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1327,12 +1324,12 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="5" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="1"/>
@@ -1340,12 +1337,12 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="1"/>
@@ -1353,12 +1350,12 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="1"/>
@@ -1366,12 +1363,12 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="1"/>
@@ -1379,7 +1376,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1392,12 +1389,12 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="1"/>
@@ -1405,12 +1402,12 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="1"/>
@@ -1418,12 +1415,12 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="1"/>
@@ -1431,7 +1428,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1444,12 +1441,12 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="1"/>
@@ -1457,7 +1454,7 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1470,12 +1467,12 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="1"/>
@@ -1483,12 +1480,12 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B26" s="11"/>
       <c r="C26" s="7"/>
@@ -1496,7 +1493,7 @@
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1516,170 +1513,170 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
         <v>27</v>
-      </c>
-      <c r="B1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1703,461 +1700,461 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>31</v>
-      </c>
-      <c r="D1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="36" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="37" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="38" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="39" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="40" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="42" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="43" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="44" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="45" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="46" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D46" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="47" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="48" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="51" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="53" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D53" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="55" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="56" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="57" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D57" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Help mark in Home Page
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/TestData/testData.xlsx
+++ b/src/main/java/com/qa/TestData/testData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{17BF5642-E7A1-4A85-97B6-36B048F52CCB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{81AABF16-9D16-4F49-A12F-4FC34914F27D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10845" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="152">
   <si>
     <t>Full Name</t>
   </si>
@@ -99,9 +99,6 @@
     <t>This is a valid All Fields scenario. It is supposed give a toast message "STP created successfully!"</t>
   </si>
   <si>
-    <t>On Par</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
@@ -462,16 +459,25 @@
     <t>application12</t>
   </si>
   <si>
-    <t>FullName117016</t>
-  </si>
-  <si>
-    <t>Short117016</t>
-  </si>
-  <si>
-    <t>FullName217016</t>
-  </si>
-  <si>
-    <t>Short217016</t>
+    <t>Ferrari19</t>
+  </si>
+  <si>
+    <t>Ferrari141</t>
+  </si>
+  <si>
+    <t>On Par with competation</t>
+  </si>
+  <si>
+    <t>FullName121012</t>
+  </si>
+  <si>
+    <t>FullName221012</t>
+  </si>
+  <si>
+    <t>Short121012</t>
+  </si>
+  <si>
+    <t>Short221012</t>
   </si>
 </sst>
 </file>
@@ -1103,7 +1109,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1145,17 +1151,17 @@
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1164,19 +1170,19 @@
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -1200,24 +1206,24 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H5" s="22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1230,15 +1236,15 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="1"/>
@@ -1272,7 +1278,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1285,12 +1291,12 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="1"/>
@@ -1298,12 +1304,12 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="1"/>
@@ -1311,7 +1317,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1324,12 +1330,12 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="1"/>
@@ -1337,12 +1343,12 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="1"/>
@@ -1350,12 +1356,12 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="1"/>
@@ -1363,12 +1369,12 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="1"/>
@@ -1376,7 +1382,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1389,12 +1395,12 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="1"/>
@@ -1402,12 +1408,12 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="1"/>
@@ -1415,12 +1421,12 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="1"/>
@@ -1428,7 +1434,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1441,12 +1447,12 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="1"/>
@@ -1454,7 +1460,7 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1467,12 +1473,12 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="1"/>
@@ -1480,12 +1486,12 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B26" s="11"/>
       <c r="C26" s="7"/>
@@ -1493,7 +1499,7 @@
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="8" t="s">
-        <v>25</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1506,177 +1512,177 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:A21"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
         <v>26</v>
-      </c>
-      <c r="B1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1688,8 +1694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C087CA4-610E-4A04-B4C6-323422E74A89}">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D57"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1700,24 +1706,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>30</v>
-      </c>
-      <c r="D1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
@@ -1728,10 +1734,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
@@ -1742,10 +1748,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
@@ -1756,10 +1762,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
@@ -1770,10 +1776,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C6" t="s">
         <v>19</v>
@@ -1784,10 +1790,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
@@ -1798,10 +1804,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
@@ -1812,10 +1818,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C9" t="s">
         <v>19</v>
@@ -1826,10 +1832,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C10" t="s">
         <v>19</v>
@@ -1840,10 +1846,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C11" t="s">
         <v>19</v>
@@ -1854,10 +1860,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C12" t="s">
         <v>19</v>
@@ -1868,10 +1874,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C13" t="s">
         <v>19</v>
@@ -1882,10 +1888,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C14" t="s">
         <v>19</v>
@@ -1896,10 +1902,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C15" t="s">
         <v>19</v>
@@ -1910,10 +1916,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C16" t="s">
         <v>19</v>
@@ -1924,10 +1930,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C17" t="s">
         <v>19</v>
@@ -1938,10 +1944,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C18" t="s">
         <v>19</v>
@@ -1952,10 +1958,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C19" t="s">
         <v>19</v>
@@ -1973,6 +1979,15 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>145</v>
+      </c>
+      <c r="B21" t="s">
+        <v>146</v>
+      </c>
+      <c r="C21" t="s">
+        <v>19</v>
+      </c>
       <c r="D21" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
Discard and My STPs
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/TestData/testData.xlsx
+++ b/src/main/java/com/qa/TestData/testData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{81AABF16-9D16-4F49-A12F-4FC34914F27D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{16C10240-C2CF-449A-A78A-88EFD3BF6D86}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10845" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -468,16 +468,16 @@
     <t>On Par with competation</t>
   </si>
   <si>
-    <t>FullName121012</t>
-  </si>
-  <si>
-    <t>FullName221012</t>
-  </si>
-  <si>
-    <t>Short121012</t>
-  </si>
-  <si>
-    <t>Short221012</t>
+    <t>FullName122011</t>
+  </si>
+  <si>
+    <t>Short122011</t>
+  </si>
+  <si>
+    <t>FullName222011</t>
+  </si>
+  <si>
+    <t>Short222011</t>
   </si>
 </sst>
 </file>
@@ -1109,7 +1109,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1161,7 +1161,7 @@
         <v>148</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1179,7 +1179,7 @@
         <v>63</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>151</v>

</xml_diff>

<commit_message>
Revert "Revert "Uday's code""
This reverts commit 8df929fb7a77ab120940f60664b7ff42e57529e9.
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/TestData/testData.xlsx
+++ b/src/main/java/com/qa/TestData/testData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A882A0C4-440F-497F-B710-B5253D05FCF8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{37182583-27E5-4BBE-976F-1C462908061B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14985" windowHeight="3945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -474,16 +474,16 @@
     <t>Publications By Merck/EMD</t>
   </si>
   <si>
-    <t>FullName118017</t>
-  </si>
-  <si>
-    <t>Short128017</t>
-  </si>
-  <si>
-    <t>FullName218017</t>
-  </si>
-  <si>
-    <t>Short218017</t>
+    <t>FullName121014</t>
+  </si>
+  <si>
+    <t>Short121014</t>
+  </si>
+  <si>
+    <t>FullName221014</t>
+  </si>
+  <si>
+    <t>Short221014</t>
   </si>
 </sst>
 </file>
@@ -1115,7 +1115,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1518,7 +1518,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D2" sqref="D2:D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Revert "Revert "Revert "Uday's code"""
This reverts commit 4abd7c8650163925349054bffca8e1c5948a5073.
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/TestData/testData.xlsx
+++ b/src/main/java/com/qa/TestData/testData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{37182583-27E5-4BBE-976F-1C462908061B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A882A0C4-440F-497F-B710-B5253D05FCF8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14985" windowHeight="3945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -474,16 +474,16 @@
     <t>Publications By Merck/EMD</t>
   </si>
   <si>
-    <t>FullName121014</t>
-  </si>
-  <si>
-    <t>Short121014</t>
-  </si>
-  <si>
-    <t>FullName221014</t>
-  </si>
-  <si>
-    <t>Short221014</t>
+    <t>FullName118017</t>
+  </si>
+  <si>
+    <t>Short128017</t>
+  </si>
+  <si>
+    <t>FullName218017</t>
+  </si>
+  <si>
+    <t>Short218017</t>
   </si>
 </sst>
 </file>
@@ -1115,7 +1115,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1518,7 +1518,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D57"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Reset the priorities of test case Execution
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/TestData/testData.xlsx
+++ b/src/main/java/com/qa/TestData/testData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8513B071-596B-4EFC-A1BD-E63253A8F569}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{70316DE7-C1AD-417D-888B-32B43383FB22}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14985" windowHeight="3945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -474,16 +474,16 @@
     <t>Publications By Merck/EMD</t>
   </si>
   <si>
-    <t>FullName122013</t>
-  </si>
-  <si>
-    <t>FullName222013</t>
-  </si>
-  <si>
-    <t>Short222013</t>
-  </si>
-  <si>
-    <t>Short122013</t>
+    <t>FullName122015</t>
+  </si>
+  <si>
+    <t>Short122015</t>
+  </si>
+  <si>
+    <t>FullName222014</t>
+  </si>
+  <si>
+    <t>Short222014</t>
   </si>
 </sst>
 </file>
@@ -1115,7 +1115,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1167,7 +1167,7 @@
         <v>150</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1185,10 +1185,10 @@
         <v>66</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>153</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.25">

</xml_diff>